<commit_message>
02 march 2023 dsr
02 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -66,18 +66,30 @@
   <si>
     <t>watch video from youtube about the agm-core of angular N understand what's going on</t>
   </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>try find the solution from google N does not work N other methods search from the google like parallel api N dependent api's in angular</t>
+  </si>
+  <si>
+    <t>I discussed with Faizan and showed the problem to Sandeep N try to figure out the Solution N apply all the changes N see the Changes On localhost</t>
+  </si>
+  <si>
+    <t>try to figure out the solution from youtube videos like forkJoin N shared Module</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="h:mm"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="h:mm"/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -110,39 +122,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,15 +146,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,9 +160,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,15 +190,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -224,15 +214,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,7 +245,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,13 +285,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,151 +447,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,20 +489,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,50 +536,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,155 +557,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -730,13 +742,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -747,6 +759,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,7 +1099,7 @@
   <dimension ref="A3:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1288,100 +1318,140 @@
       <c r="N15" s="9"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3">
+        <v>44987</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.430555555555556</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="9"/>
@@ -2040,16 +2110,28 @@
       <c r="N62" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="21">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
     <mergeCell ref="F11:N11"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="F13:N13"/>
+    <mergeCell ref="F16:N16"/>
+    <mergeCell ref="F21:N21"/>
     <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A17:A21"/>
     <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="D3:K4"/>
+    <mergeCell ref="F17:N18"/>
+    <mergeCell ref="F19:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
03 March 2023 dsr
03 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -77,6 +77,27 @@
   </si>
   <si>
     <t>try to figure out the solution from youtube videos like forkJoin N shared Module</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>WBX-4237</t>
+  </si>
+  <si>
+    <t>DSM</t>
+  </si>
+  <si>
+    <t>Seach from the google more loading bar issue N undderstand the code and try to apply them for issue fix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch youtube video for the issue related like parallel api how  works together N try to solve the issue </t>
+  </si>
+  <si>
+    <t>WBX-4206</t>
+  </si>
+  <si>
+    <t>This time i try to fix the bug N applied the code logics N raise the PR for reviewing for stuck login page at the dashboard admin N merchant both</t>
   </si>
 </sst>
 </file>
@@ -85,13 +106,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="h:mm"/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="181" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,15 +144,38 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,10 +189,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -167,9 +220,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,11 +241,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -198,19 +257,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -228,35 +286,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -285,13 +314,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,13 +362,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,13 +398,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,109 +452,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,17 +518,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,6 +538,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,7 +576,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,9 +598,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,166 +615,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,40 +771,31 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1098,8 +1118,8 @@
   <sheetPr/>
   <dimension ref="A3:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1376,18 +1396,18 @@
     <row r="18" spans="1:14">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="3"/>
@@ -1416,27 +1436,27 @@
     <row r="20" spans="1:14">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="5">
-        <v>0.208333333333333</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="E21" s="5">
         <v>0.270833333333333</v>
@@ -1486,132 +1506,168 @@
       <c r="N23" s="9"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
+      <c r="A25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3">
+        <v>44988</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="9"/>
@@ -2110,7 +2166,7 @@
       <c r="N62" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="34">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -2119,19 +2175,32 @@
     <mergeCell ref="F13:N13"/>
     <mergeCell ref="F16:N16"/>
     <mergeCell ref="F21:N21"/>
+    <mergeCell ref="F24:N24"/>
+    <mergeCell ref="F25:N25"/>
+    <mergeCell ref="F30:N30"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A25:A30"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B25:B30"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="D3:K4"/>
     <mergeCell ref="F17:N18"/>
     <mergeCell ref="F19:N20"/>
+    <mergeCell ref="F26:N27"/>
+    <mergeCell ref="F28:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
06 march 2023 dsr
06 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -98,6 +98,36 @@
   </si>
   <si>
     <t>This time i try to fix the bug N applied the code logics N raise the PR for reviewing for stuck login page at the dashboard admin N merchant both</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Weekend Holiday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>WBX-4285</t>
+  </si>
+  <si>
+    <t>Walkthrough the code of loginhandler N understand the isssue what's going there apply different methods here</t>
+  </si>
+  <si>
+    <t>walkthrough the onsubmit method understand the issue here why problem is here</t>
+  </si>
+  <si>
+    <t>WBX-4264</t>
+  </si>
+  <si>
+    <t>try all solution applied one of them is when user active N show error msg user not found</t>
+  </si>
+  <si>
+    <t>Holi celebration</t>
   </si>
 </sst>
 </file>
@@ -105,12 +135,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="h:mm"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="181" formatCode="h:mm"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -152,30 +182,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,76 +226,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,14 +244,74 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,43 +350,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,7 +482,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,19 +500,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,86 +510,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -518,11 +548,182 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,6 +743,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -557,41 +767,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -606,164 +786,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -771,13 +942,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -788,7 +959,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,6 +967,63 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="12" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="13" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="14" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1118,8 +1346,8 @@
   <sheetPr/>
   <dimension ref="A3:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1686,164 +1914,156 @@
       <c r="N32" s="9"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
+      <c r="A33" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="28"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="A34" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="17">
+        <v>44989</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="29"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="30"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="31"/>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
+      <c r="A39" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="28"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
+      <c r="A40" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="17">
+        <v>44990</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="29"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="30"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="31"/>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="9"/>
@@ -1878,116 +2098,172 @@
       <c r="N44" s="9"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
+      <c r="A45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
+      <c r="A46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="3">
+        <v>44991</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E47" s="10">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E49" s="10">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="10">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E50" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
-      <c r="N51" s="9"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="9"/>
@@ -2166,7 +2442,7 @@
       <c r="N62" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="53">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -2178,29 +2454,48 @@
     <mergeCell ref="F24:N24"/>
     <mergeCell ref="F25:N25"/>
     <mergeCell ref="F30:N30"/>
+    <mergeCell ref="C33:N33"/>
+    <mergeCell ref="C39:N39"/>
+    <mergeCell ref="F45:N45"/>
+    <mergeCell ref="F46:N46"/>
+    <mergeCell ref="F49:N49"/>
+    <mergeCell ref="F50:N50"/>
+    <mergeCell ref="F51:N51"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A46:A51"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B46:B51"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C47:C48"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D47:D48"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E47:E48"/>
     <mergeCell ref="D3:K4"/>
     <mergeCell ref="F17:N18"/>
     <mergeCell ref="F19:N20"/>
     <mergeCell ref="F26:N27"/>
     <mergeCell ref="F28:N29"/>
+    <mergeCell ref="C34:N36"/>
+    <mergeCell ref="C40:N42"/>
+    <mergeCell ref="F47:N48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
08 march 2023 dsr
08 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -128,6 +128,33 @@
   </si>
   <si>
     <t>Holi celebration</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>On the occasion of Holi, Holiday</t>
+  </si>
+  <si>
+    <t>WBX-4203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">walkthrough the dashboard module N home module N wallkthrough the all modules code regarding the issue apply different approaches </t>
+  </si>
+  <si>
+    <t>R&amp;D for viewing dashboard issue</t>
+  </si>
+  <si>
+    <t>WBX-4297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applied translation on community module </t>
+  </si>
+  <si>
+    <t>LMDI-37</t>
+  </si>
+  <si>
+    <t>Women's Day Celebration</t>
   </si>
 </sst>
 </file>
@@ -135,12 +162,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="h:mm"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="h:mm"/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -181,6 +208,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -195,80 +238,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -290,14 +264,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,12 +293,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -356,157 +383,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,15 +712,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,17 +731,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -743,11 +755,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,6 +787,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -778,163 +807,161 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -942,13 +969,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -959,7 +986,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -980,7 +1007,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -992,7 +1019,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1004,7 +1031,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1023,6 +1050,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1344,10 +1374,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N62"/>
+  <dimension ref="A3:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="Q66" sqref="Q66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2298,68 +2328,80 @@
       <c r="N53" s="9"/>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
+      <c r="A54" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="28"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
-      <c r="N55" s="9"/>
+      <c r="A55" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="17">
+        <v>44992</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="29"/>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="9"/>
-      <c r="N56" s="9"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
+      <c r="K56" s="23"/>
+      <c r="L56" s="23"/>
+      <c r="M56" s="23"/>
+      <c r="N56" s="30"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="9"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="27"/>
+      <c r="N57" s="31"/>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" s="9"/>
@@ -2394,55 +2436,199 @@
       <c r="N59" s="9"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
-      <c r="M60" s="9"/>
-      <c r="N60" s="9"/>
+      <c r="A60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
-      <c r="N61" s="9"/>
+      <c r="A61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="3">
+        <v>44993</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="5">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" s="10">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E62" s="10">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11"/>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E64" s="10">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" s="5">
+        <v>0.1875</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="32"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66" s="5">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="E66" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="32"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D67" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E67" s="5">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="69">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -2461,33 +2647,47 @@
     <mergeCell ref="F49:N49"/>
     <mergeCell ref="F50:N50"/>
     <mergeCell ref="F51:N51"/>
+    <mergeCell ref="C54:N54"/>
+    <mergeCell ref="F60:N60"/>
+    <mergeCell ref="F61:N61"/>
+    <mergeCell ref="F64:N64"/>
+    <mergeCell ref="F65:N65"/>
+    <mergeCell ref="F66:N66"/>
+    <mergeCell ref="F67:N67"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A25:A30"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A46:A51"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A61:A67"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B25:B30"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="B46:B51"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B61:B67"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C62:C63"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D62:D63"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E47:E48"/>
+    <mergeCell ref="E62:E63"/>
     <mergeCell ref="D3:K4"/>
     <mergeCell ref="F17:N18"/>
     <mergeCell ref="F19:N20"/>
@@ -2496,6 +2696,8 @@
     <mergeCell ref="C34:N36"/>
     <mergeCell ref="C40:N42"/>
     <mergeCell ref="F47:N48"/>
+    <mergeCell ref="C55:N57"/>
+    <mergeCell ref="F62:N63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
08 march 2023 dsr update
08 march 2023 dsr update
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -162,12 +162,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="h:mm"/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="h:mm"/>
+    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -208,9 +208,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,15 +230,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,6 +291,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -262,32 +307,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,43 +338,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,13 +383,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,139 +521,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,6 +712,78 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,60 +805,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -795,173 +813,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -969,13 +969,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -986,7 +986,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1007,7 +1007,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1019,7 +1019,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1031,7 +1031,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1050,9 +1050,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1376,8 +1373,8 @@
   <sheetPr/>
   <dimension ref="A3:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Q66" sqref="Q66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2561,8 +2558,8 @@
       <c r="C65" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D65" s="5">
-        <v>0.1875</v>
+      <c r="D65" s="10">
+        <v>0.166666666666667</v>
       </c>
       <c r="E65" s="5">
         <v>0.229166666666667</v>
@@ -2580,8 +2577,8 @@
       <c r="N65" s="6"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="32"/>
-      <c r="B66" s="32"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
       <c r="C66" s="7" t="s">
         <v>45</v>
       </c>
@@ -2604,8 +2601,8 @@
       <c r="N66" s="6"/>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="32"/>
-      <c r="B67" s="32"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
       <c r="C67" s="7" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
09 march 2023 dsr
09 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -155,6 +155,27 @@
   </si>
   <si>
     <t>Women's Day Celebration</t>
+  </si>
+  <si>
+    <t>Add translation on community module</t>
+  </si>
+  <si>
+    <t>office cleaning</t>
+  </si>
+  <si>
+    <t>R&amp;D on new tab for home module along with dashboard modules</t>
+  </si>
+  <si>
+    <t>applied different approaches on the issue tried to solve the issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on the reopen ticket try to fix new issues </t>
+  </si>
+  <si>
+    <t>WBX-4298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applied translation on announcement module </t>
   </si>
 </sst>
 </file>
@@ -162,11 +183,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="h:mm"/>
-    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="179" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="180" formatCode="h:mm"/>
     <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -208,8 +229,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,6 +239,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,9 +259,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,28 +268,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,11 +282,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -307,8 +328,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -329,20 +351,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -389,139 +410,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,11 +737,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,21 +801,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -799,6 +811,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -822,142 +843,142 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -969,26 +990,26 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1007,7 +1028,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1019,7 +1040,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1031,7 +1052,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1371,10 +1392,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N67"/>
+  <dimension ref="A3:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="S65" sqref="S65"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2624,8 +2645,208 @@
       <c r="M67" s="6"/>
       <c r="N67" s="6"/>
     </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="3">
+        <v>44994</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="5">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+      <c r="N72" s="11"/>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="5">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="11"/>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="11"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="E74" s="10">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="11"/>
+      <c r="K74" s="11"/>
+      <c r="L74" s="11"/>
+      <c r="M74" s="11"/>
+      <c r="N74" s="11"/>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" s="10">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E76" s="10">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77" s="10">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E77" s="5">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="69">
+  <mergeCells count="79">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -2651,6 +2872,14 @@
     <mergeCell ref="F65:N65"/>
     <mergeCell ref="F66:N66"/>
     <mergeCell ref="F67:N67"/>
+    <mergeCell ref="F70:N70"/>
+    <mergeCell ref="F71:N71"/>
+    <mergeCell ref="F72:N72"/>
+    <mergeCell ref="F73:N73"/>
+    <mergeCell ref="F74:N74"/>
+    <mergeCell ref="F75:N75"/>
+    <mergeCell ref="F76:N76"/>
+    <mergeCell ref="F77:N77"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A25:A30"/>
@@ -2659,6 +2888,7 @@
     <mergeCell ref="A46:A51"/>
     <mergeCell ref="A55:A57"/>
     <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A71:A77"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B25:B30"/>
@@ -2667,6 +2897,7 @@
     <mergeCell ref="B46:B51"/>
     <mergeCell ref="B55:B57"/>
     <mergeCell ref="B61:B67"/>
+    <mergeCell ref="B71:B77"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C26:C27"/>

</xml_diff>

<commit_message>
10 march 2023 dsr
10 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="59">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -176,6 +176,21 @@
   </si>
   <si>
     <t xml:space="preserve">applied translation on announcement module </t>
+  </si>
+  <si>
+    <t>R&amp;D for logged user open new tab first open home page  sometimes then dashboard page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried different approaches N see the changes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">check the code implementation right now is show login page along with dashboard </t>
+  </si>
+  <si>
+    <t>WBX-4284</t>
+  </si>
+  <si>
+    <t>ashwani's code working and code implementation is reviewed</t>
   </si>
 </sst>
 </file>
@@ -183,12 +198,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="180" formatCode="h:mm"/>
-    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="h:mm"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -229,14 +244,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -251,16 +258,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,16 +274,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,17 +312,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,18 +335,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -351,8 +358,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,7 +419,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,13 +431,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,19 +503,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,31 +539,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,43 +551,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,19 +563,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,6 +808,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -823,166 +849,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -990,13 +1005,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1007,7 +1022,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1028,7 +1043,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1040,7 +1055,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,7 +1067,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1073,6 +1088,7 @@
     <xf numFmtId="20" fontId="4" fillId="6" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,10 +1408,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N77"/>
+  <dimension ref="A3:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="P75" sqref="P75"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="Q84" sqref="Q84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2845,8 +2861,200 @@
       <c r="M77" s="6"/>
       <c r="N77" s="6"/>
     </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+    </row>
+    <row r="81" spans="1:14">
+      <c r="A81" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="3">
+        <v>44995</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D81" s="5">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E81" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E82" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="L83" s="11"/>
+      <c r="M83" s="11"/>
+      <c r="N83" s="11"/>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E84" s="5">
+        <v>0.1875</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="11"/>
+      <c r="K84" s="11"/>
+      <c r="L84" s="11"/>
+      <c r="M84" s="11"/>
+      <c r="N84" s="11"/>
+    </row>
+    <row r="85" spans="1:14">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="5">
+        <v>0.1875</v>
+      </c>
+      <c r="E85" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+    </row>
+    <row r="86" spans="1:14">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="E86" s="5">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+    </row>
+    <row r="87" spans="1:14">
+      <c r="A87" s="32"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="32"/>
+      <c r="G87" s="32"/>
+      <c r="H87" s="32"/>
+      <c r="I87" s="32"/>
+      <c r="J87" s="32"/>
+      <c r="K87" s="32"/>
+      <c r="L87" s="32"/>
+      <c r="M87" s="32"/>
+      <c r="N87" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="89">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -2880,6 +3088,14 @@
     <mergeCell ref="F75:N75"/>
     <mergeCell ref="F76:N76"/>
     <mergeCell ref="F77:N77"/>
+    <mergeCell ref="F80:N80"/>
+    <mergeCell ref="F81:N81"/>
+    <mergeCell ref="F82:N82"/>
+    <mergeCell ref="F83:N83"/>
+    <mergeCell ref="F84:N84"/>
+    <mergeCell ref="F85:N85"/>
+    <mergeCell ref="F86:N86"/>
+    <mergeCell ref="F87:N87"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A25:A30"/>
@@ -2889,6 +3105,7 @@
     <mergeCell ref="A55:A57"/>
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="A71:A77"/>
+    <mergeCell ref="A81:A86"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B25:B30"/>
@@ -2898,6 +3115,7 @@
     <mergeCell ref="B55:B57"/>
     <mergeCell ref="B61:B67"/>
     <mergeCell ref="B71:B77"/>
+    <mergeCell ref="B81:B86"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C26:C27"/>

</xml_diff>

<commit_message>
13 march 2023 dsr
13 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -191,6 +191,27 @@
   </si>
   <si>
     <t>ashwani's code working and code implementation is reviewed</t>
+  </si>
+  <si>
+    <t>WBX-4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on the issue where is logged user open new tab firs sometime splash screen is appear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">walkthrough the given tickets and their modules N try to figure out the solutions </t>
+  </si>
+  <si>
+    <t>WBX-4271</t>
+  </si>
+  <si>
+    <t>applied greet on the user by created by super admin</t>
+  </si>
+  <si>
+    <t>WBX4296</t>
+  </si>
+  <si>
+    <t>communities downvote issue understand what's going on here</t>
   </si>
 </sst>
 </file>
@@ -198,12 +219,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="h:mm"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="181" formatCode="h:mm"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -244,8 +265,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,38 +297,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,16 +318,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -335,18 +342,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -367,14 +388,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,43 +440,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,49 +500,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,7 +518,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,13 +542,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,19 +572,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,21 +773,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -808,20 +814,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -843,6 +853,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -852,15 +873,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -870,130 +891,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1005,26 +1026,26 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1043,7 +1064,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1055,7 +1076,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1067,7 +1088,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1408,10 +1429,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N87"/>
+  <dimension ref="A3:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="Q84" sqref="Q84"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="P106" sqref="P106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3038,23 +3059,343 @@
       <c r="N86" s="6"/>
     </row>
     <row r="87" spans="1:14">
-      <c r="A87" s="32"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="32"/>
-      <c r="H87" s="32"/>
-      <c r="I87" s="32"/>
-      <c r="J87" s="32"/>
-      <c r="K87" s="32"/>
-      <c r="L87" s="32"/>
-      <c r="M87" s="32"/>
-      <c r="N87" s="32"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
+    </row>
+    <row r="89" spans="1:14">
+      <c r="A89" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="15"/>
+      <c r="M89" s="15"/>
+      <c r="N89" s="28"/>
+    </row>
+    <row r="90" spans="1:14">
+      <c r="A90" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" s="17">
+        <v>44996</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="19"/>
+      <c r="I90" s="19"/>
+      <c r="J90" s="19"/>
+      <c r="K90" s="19"/>
+      <c r="L90" s="19"/>
+      <c r="M90" s="19"/>
+      <c r="N90" s="29"/>
+    </row>
+    <row r="91" spans="1:14">
+      <c r="A91" s="20"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
+      <c r="I91" s="23"/>
+      <c r="J91" s="23"/>
+      <c r="K91" s="23"/>
+      <c r="L91" s="23"/>
+      <c r="M91" s="23"/>
+      <c r="N91" s="30"/>
+    </row>
+    <row r="92" spans="1:14">
+      <c r="A92" s="24"/>
+      <c r="B92" s="25"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="27"/>
+      <c r="I92" s="27"/>
+      <c r="J92" s="27"/>
+      <c r="K92" s="27"/>
+      <c r="L92" s="27"/>
+      <c r="M92" s="27"/>
+      <c r="N92" s="31"/>
+    </row>
+    <row r="95" spans="1:14">
+      <c r="A95" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="15"/>
+      <c r="N95" s="28"/>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="A96" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="17">
+        <v>44997</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
+      <c r="J96" s="19"/>
+      <c r="K96" s="19"/>
+      <c r="L96" s="19"/>
+      <c r="M96" s="19"/>
+      <c r="N96" s="29"/>
+    </row>
+    <row r="97" spans="1:14">
+      <c r="A97" s="20"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
+      <c r="H97" s="23"/>
+      <c r="I97" s="23"/>
+      <c r="J97" s="23"/>
+      <c r="K97" s="23"/>
+      <c r="L97" s="23"/>
+      <c r="M97" s="23"/>
+      <c r="N97" s="30"/>
+    </row>
+    <row r="98" spans="1:14">
+      <c r="A98" s="24"/>
+      <c r="B98" s="25"/>
+      <c r="C98" s="26"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="27"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="27"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="27"/>
+      <c r="M98" s="27"/>
+      <c r="N98" s="31"/>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B102" s="3">
+        <v>44998</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D102" s="5">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E102" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E103" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E104" s="5">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F104" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G104" s="11"/>
+      <c r="H104" s="11"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="11"/>
+      <c r="K104" s="11"/>
+      <c r="L104" s="11"/>
+      <c r="M104" s="11"/>
+      <c r="N104" s="11"/>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D105" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E105" s="5">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F105" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G105" s="11"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="11"/>
+      <c r="K105" s="11"/>
+      <c r="L105" s="11"/>
+      <c r="M105" s="11"/>
+      <c r="N105" s="11"/>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D106" s="5">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E106" s="5">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="A107" s="32"/>
+      <c r="B107" s="32"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="32"/>
+      <c r="F107" s="32"/>
+      <c r="G107" s="32"/>
+      <c r="H107" s="32"/>
+      <c r="I107" s="32"/>
+      <c r="J107" s="32"/>
+      <c r="K107" s="32"/>
+      <c r="L107" s="32"/>
+      <c r="M107" s="32"/>
+      <c r="N107" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="89">
+  <mergeCells count="106">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -3096,6 +3437,15 @@
     <mergeCell ref="F85:N85"/>
     <mergeCell ref="F86:N86"/>
     <mergeCell ref="F87:N87"/>
+    <mergeCell ref="C89:N89"/>
+    <mergeCell ref="C95:N95"/>
+    <mergeCell ref="F101:N101"/>
+    <mergeCell ref="F102:N102"/>
+    <mergeCell ref="F103:N103"/>
+    <mergeCell ref="F104:N104"/>
+    <mergeCell ref="F105:N105"/>
+    <mergeCell ref="F106:N106"/>
+    <mergeCell ref="F107:N107"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A25:A30"/>
@@ -3106,6 +3456,9 @@
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="A71:A77"/>
     <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A102:A106"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B25:B30"/>
@@ -3116,6 +3469,9 @@
     <mergeCell ref="B61:B67"/>
     <mergeCell ref="B71:B77"/>
     <mergeCell ref="B81:B86"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="B102:B106"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C26:C27"/>
@@ -3144,6 +3500,8 @@
     <mergeCell ref="F47:N48"/>
     <mergeCell ref="C55:N57"/>
     <mergeCell ref="F62:N63"/>
+    <mergeCell ref="C90:N92"/>
+    <mergeCell ref="C96:N98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
14 march 2023 dsr
14 march 2023 dsr
</commit_message>
<xml_diff>
--- a/03_march/march2023.xlsx
+++ b/03_march/march2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="69">
   <si>
     <t>Start March Month 2023</t>
   </si>
@@ -196,7 +196,7 @@
     <t>WBX-4321</t>
   </si>
   <si>
-    <t xml:space="preserve">work on the issue where is logged user open new tab firs sometime splash screen is appear </t>
+    <t xml:space="preserve">work on the issue where is logged user open new tab first sometime splash screen is appear </t>
   </si>
   <si>
     <t xml:space="preserve">walkthrough the given tickets and their modules N try to figure out the solutions </t>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>communities downvote issue understand what's going on here</t>
+  </si>
+  <si>
+    <t>download android local build N setup on smartphone N check is working or not N api is not w</t>
+  </si>
+  <si>
+    <t>walkthrough the postlikeunlike modules N functions N  figure out the problem</t>
+  </si>
+  <si>
+    <t>apply different approaches N try them into the apis check the changes on the like N dislike console screen</t>
   </si>
 </sst>
 </file>
@@ -219,12 +228,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="h:mm"/>
+    <numFmt numFmtId="176" formatCode="h:mm"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -265,24 +274,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,11 +296,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -319,18 +335,26 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -351,37 +375,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,7 +389,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -440,120 +449,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -566,7 +461,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,19 +539,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,6 +782,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -814,6 +838,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -821,17 +856,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,175 +879,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1026,13 +1035,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1043,7 +1052,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1064,7 +1073,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="6" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1076,7 +1085,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="6" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1088,7 +1097,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="6" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="6" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1109,7 +1118,6 @@
     <xf numFmtId="20" fontId="4" fillId="6" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,10 +1437,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N107"/>
+  <dimension ref="A3:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="P106" sqref="P106"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="O113" sqref="O113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3379,23 +3387,167 @@
       <c r="N106" s="6"/>
     </row>
     <row r="107" spans="1:14">
-      <c r="A107" s="32"/>
-      <c r="B107" s="32"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="32"/>
-      <c r="H107" s="32"/>
-      <c r="I107" s="32"/>
-      <c r="J107" s="32"/>
-      <c r="K107" s="32"/>
-      <c r="L107" s="32"/>
-      <c r="M107" s="32"/>
-      <c r="N107" s="32"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
+      <c r="L107" s="9"/>
+      <c r="M107" s="9"/>
+      <c r="N107" s="9"/>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="2"/>
+      <c r="N109" s="2"/>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="A110" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B110" s="3">
+        <v>44999</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D110" s="5">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E110" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
+      <c r="N110" s="6"/>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="A111" s="3"/>
+      <c r="B111" s="3"/>
+      <c r="C111" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D111" s="5">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E111" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="6"/>
+      <c r="N111" s="6"/>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
+      <c r="C112" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="E112" s="5">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
+      <c r="I112" s="11"/>
+      <c r="J112" s="11"/>
+      <c r="K112" s="11"/>
+      <c r="L112" s="11"/>
+      <c r="M112" s="11"/>
+      <c r="N112" s="11"/>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D113" s="10">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E113" s="10">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F113" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G113" s="11"/>
+      <c r="H113" s="11"/>
+      <c r="I113" s="11"/>
+      <c r="J113" s="11"/>
+      <c r="K113" s="11"/>
+      <c r="L113" s="11"/>
+      <c r="M113" s="11"/>
+      <c r="N113" s="11"/>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="3"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="11"/>
+      <c r="K114" s="11"/>
+      <c r="L114" s="11"/>
+      <c r="M114" s="11"/>
+      <c r="N114" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="106">
+  <mergeCells count="116">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -3446,6 +3598,10 @@
     <mergeCell ref="F105:N105"/>
     <mergeCell ref="F106:N106"/>
     <mergeCell ref="F107:N107"/>
+    <mergeCell ref="F109:N109"/>
+    <mergeCell ref="F110:N110"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="F112:N112"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A25:A30"/>
@@ -3459,6 +3615,7 @@
     <mergeCell ref="A90:A92"/>
     <mergeCell ref="A96:A98"/>
     <mergeCell ref="A102:A106"/>
+    <mergeCell ref="A110:A114"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B25:B30"/>
@@ -3472,24 +3629,28 @@
     <mergeCell ref="B90:B92"/>
     <mergeCell ref="B96:B98"/>
     <mergeCell ref="B102:B106"/>
+    <mergeCell ref="B110:B114"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C113:C114"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D113:D114"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="E62:E63"/>
+    <mergeCell ref="E113:E114"/>
     <mergeCell ref="D3:K4"/>
     <mergeCell ref="F17:N18"/>
     <mergeCell ref="F19:N20"/>
@@ -3502,6 +3663,7 @@
     <mergeCell ref="F62:N63"/>
     <mergeCell ref="C90:N92"/>
     <mergeCell ref="C96:N98"/>
+    <mergeCell ref="F113:N114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>